<commit_message>
Added masses to database
Added particle masses to the XLSX database that will be used to update the database of javascript objects in an array.
</commit_message>
<xml_diff>
--- a/ccc-simulation-p5js/assets/chemdb.xlsx
+++ b/ccc-simulation-p5js/assets/chemdb.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="684">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -659,9 +659,6 @@
   </si>
   <si>
     <t xml:space="preserve">ethene</t>
-  </si>
-  <si>
-    <t xml:space="preserve">filenames.txt</t>
   </si>
   <si>
     <t xml:space="preserve">Fluoride.svg</t>
@@ -2089,6 +2086,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2148,9 +2146,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2170,19 +2172,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F228"/>
+  <dimension ref="A1:F227"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="F121" activeCellId="0" sqref="F121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.47959183673469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.1632653061224"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.6887755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.1275510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.32142857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.7857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2276,6 +2278,9 @@
         <f aca="false">RIGHT(B5,3)</f>
         <v>svg</v>
       </c>
+      <c r="F5" s="1" t="n">
+        <v>59.04</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -2294,6 +2299,9 @@
         <f aca="false">RIGHT(B6,3)</f>
         <v>svg</v>
       </c>
+      <c r="F6" s="0" t="n">
+        <v>60.05</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -2312,6 +2320,9 @@
         <f aca="false">RIGHT(B7,3)</f>
         <v>svg</v>
       </c>
+      <c r="F7" s="0" t="n">
+        <v>133.34</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -2330,6 +2341,9 @@
         <f aca="false">RIGHT(B8,3)</f>
         <v>svg</v>
       </c>
+      <c r="F8" s="1" t="n">
+        <v>26.9815</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -2348,6 +2362,9 @@
         <f aca="false">RIGHT(B9,3)</f>
         <v>svg</v>
       </c>
+      <c r="F9" s="0" t="n">
+        <v>101.96</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -2366,6 +2383,9 @@
         <f aca="false">RIGHT(B10,3)</f>
         <v>svg</v>
       </c>
+      <c r="F10" s="1" t="n">
+        <v>26.9815</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -2384,6 +2404,9 @@
         <f aca="false">RIGHT(B11,3)</f>
         <v>svg</v>
       </c>
+      <c r="F11" s="0" t="n">
+        <v>17.031</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
@@ -2402,6 +2425,9 @@
         <f aca="false">RIGHT(B12,3)</f>
         <v>svg</v>
       </c>
+      <c r="F12" s="0" t="n">
+        <v>17.031</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
@@ -2420,6 +2446,9 @@
         <f aca="false">RIGHT(B13,3)</f>
         <v>svg</v>
       </c>
+      <c r="F13" s="0" t="n">
+        <v>77.0825</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
@@ -2438,6 +2467,9 @@
         <f aca="false">RIGHT(B14,3)</f>
         <v>svg</v>
       </c>
+      <c r="F14" s="0" t="n">
+        <v>53.491</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -2456,6 +2488,9 @@
         <f aca="false">RIGHT(B15,3)</f>
         <v>svg</v>
       </c>
+      <c r="F15" s="0" t="n">
+        <v>18.039</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
@@ -2474,6 +2509,9 @@
         <f aca="false">RIGHT(B16,3)</f>
         <v>svg</v>
       </c>
+      <c r="F16" s="0" t="n">
+        <v>80.043</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
@@ -2492,6 +2530,9 @@
         <f aca="false">RIGHT(B17,3)</f>
         <v>svg</v>
       </c>
+      <c r="F17" s="0" t="n">
+        <v>18.039</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
@@ -2510,6 +2551,9 @@
         <f aca="false">RIGHT(B18,3)</f>
         <v>svg</v>
       </c>
+      <c r="F18" s="0" t="n">
+        <v>143.92295</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
@@ -2528,6 +2572,9 @@
         <f aca="false">RIGHT(B19,3)</f>
         <v>svg</v>
       </c>
+      <c r="F19" s="0" t="n">
+        <v>61.0168</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
@@ -2564,6 +2611,9 @@
         <f aca="false">RIGHT(B21,3)</f>
         <v>svg</v>
       </c>
+      <c r="F21" s="0" t="n">
+        <v>10.811</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
@@ -2582,6 +2632,9 @@
         <f aca="false">RIGHT(B22,3)</f>
         <v>svg</v>
       </c>
+      <c r="F22" s="0" t="n">
+        <v>10.811</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
@@ -2600,6 +2653,9 @@
         <f aca="false">RIGHT(B23,3)</f>
         <v>svg</v>
       </c>
+      <c r="F23" s="0" t="n">
+        <v>152.61</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
@@ -2618,6 +2674,9 @@
         <f aca="false">RIGHT(B24,3)</f>
         <v>svg</v>
       </c>
+      <c r="F24" s="0" t="n">
+        <v>152.61</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
@@ -2636,6 +2695,9 @@
         <f aca="false">RIGHT(B25,3)</f>
         <v>svg</v>
       </c>
+      <c r="F25" s="0" t="n">
+        <v>117.17</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
@@ -2654,6 +2716,9 @@
         <f aca="false">RIGHT(B26,3)</f>
         <v>svg</v>
       </c>
+      <c r="F26" s="0" t="n">
+        <v>117.17</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
@@ -2672,6 +2737,9 @@
         <f aca="false">RIGHT(B27,3)</f>
         <v>svg</v>
       </c>
+      <c r="F27" s="0" t="n">
+        <v>79.904</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
@@ -2690,6 +2758,9 @@
         <f aca="false">RIGHT(B28,3)</f>
         <v>svg</v>
       </c>
+      <c r="F28" s="0" t="n">
+        <v>79.904</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
@@ -2708,6 +2779,9 @@
         <f aca="false">RIGHT(B29,3)</f>
         <v>svg</v>
       </c>
+      <c r="F29" s="0" t="n">
+        <v>79.904</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
@@ -2726,6 +2800,9 @@
         <f aca="false">RIGHT(B30,3)</f>
         <v>svg</v>
       </c>
+      <c r="F30" s="0" t="n">
+        <v>79.904</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
@@ -2744,6 +2821,9 @@
         <f aca="false">RIGHT(B31,3)</f>
         <v>svg</v>
       </c>
+      <c r="F31" s="0" t="n">
+        <v>79.904</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
@@ -2762,6 +2842,9 @@
         <f aca="false">RIGHT(B32,3)</f>
         <v>svg</v>
       </c>
+      <c r="F32" s="0" t="n">
+        <v>58.12</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
@@ -2780,6 +2863,9 @@
         <f aca="false">RIGHT(B33,3)</f>
         <v>svg</v>
       </c>
+      <c r="F33" s="0" t="n">
+        <v>56.11</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
@@ -2798,6 +2884,9 @@
         <f aca="false">RIGHT(B34,3)</f>
         <v>svg</v>
       </c>
+      <c r="F34" s="0" t="n">
+        <v>110.98</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
@@ -2816,6 +2905,9 @@
         <f aca="false">RIGHT(B35,3)</f>
         <v>svg</v>
       </c>
+      <c r="F35" s="0" t="n">
+        <v>40.078</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
@@ -2834,6 +2926,9 @@
         <f aca="false">RIGHT(B36,3)</f>
         <v>svg</v>
       </c>
+      <c r="F36" s="0" t="n">
+        <v>40.078</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
@@ -2870,6 +2965,9 @@
         <f aca="false">RIGHT(B38,3)</f>
         <v>svg</v>
       </c>
+      <c r="F38" s="0" t="n">
+        <v>60.01</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
@@ -2888,6 +2986,9 @@
         <f aca="false">RIGHT(B39,3)</f>
         <v>svg</v>
       </c>
+      <c r="F39" s="0" t="n">
+        <v>44.01</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
@@ -2906,6 +3007,9 @@
         <f aca="false">RIGHT(B40,3)</f>
         <v>svg</v>
       </c>
+      <c r="F40" s="0" t="n">
+        <v>62.03</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
@@ -2924,6 +3028,9 @@
         <f aca="false">RIGHT(B41,3)</f>
         <v>svg</v>
       </c>
+      <c r="F41" s="0" t="n">
+        <v>12.01</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
@@ -2942,6 +3049,9 @@
         <f aca="false">RIGHT(B42,3)</f>
         <v>svg</v>
       </c>
+      <c r="F42" s="0" t="n">
+        <v>28.01</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
@@ -2960,6 +3070,9 @@
         <f aca="false">RIGHT(B43,3)</f>
         <v>svg</v>
       </c>
+      <c r="F43" s="0" t="n">
+        <v>12.01</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
@@ -2996,6 +3109,9 @@
         <f aca="false">RIGHT(B45,3)</f>
         <v>svg</v>
       </c>
+      <c r="F45" s="0" t="n">
+        <v>136.907</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
@@ -3014,6 +3130,9 @@
         <f aca="false">RIGHT(B46,3)</f>
         <v>svg</v>
       </c>
+      <c r="F46" s="0" t="n">
+        <v>35.453</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
@@ -3032,6 +3151,9 @@
         <f aca="false">RIGHT(B47,3)</f>
         <v>svg</v>
       </c>
+      <c r="F47" s="0" t="n">
+        <v>35.453</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
@@ -3050,6 +3172,9 @@
         <f aca="false">RIGHT(B48,3)</f>
         <v>svg</v>
       </c>
+      <c r="F48" s="0" t="n">
+        <v>45</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
@@ -3068,6 +3193,9 @@
         <f aca="false">RIGHT(B49,3)</f>
         <v>svg</v>
       </c>
+      <c r="F49" s="0" t="n">
+        <v>35.453</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
@@ -3086,6 +3214,9 @@
         <f aca="false">RIGHT(B50,3)</f>
         <v>svg</v>
       </c>
+      <c r="F50" s="0" t="n">
+        <v>35.453</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
@@ -3104,6 +3235,9 @@
         <f aca="false">RIGHT(B51,3)</f>
         <v>svg</v>
       </c>
+      <c r="F51" s="0" t="n">
+        <v>97.46</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
@@ -3122,6 +3256,9 @@
         <f aca="false">RIGHT(B52,3)</f>
         <v>svg</v>
       </c>
+      <c r="F52" s="0" t="n">
+        <v>35.453</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
@@ -3140,6 +3277,9 @@
         <f aca="false">RIGHT(B53,3)</f>
         <v>svg</v>
       </c>
+      <c r="F53" s="0" t="n">
+        <v>151.99</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
@@ -3158,6 +3298,9 @@
         <f aca="false">RIGHT(B54,3)</f>
         <v>svg</v>
       </c>
+      <c r="F54" s="0" t="n">
+        <v>51.9961</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
@@ -3176,6 +3319,9 @@
         <f aca="false">RIGHT(B55,3)</f>
         <v>svg</v>
       </c>
+      <c r="F55" s="0" t="n">
+        <v>51.9961</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
@@ -3194,6 +3340,9 @@
         <f aca="false">RIGHT(B56,3)</f>
         <v>svg</v>
       </c>
+      <c r="F56" s="0" t="n">
+        <v>51.9961</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
@@ -3212,6 +3361,9 @@
         <f aca="false">RIGHT(B57,3)</f>
         <v>svg</v>
       </c>
+      <c r="F57" s="0" t="n">
+        <v>51.9961</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
@@ -3230,6 +3382,9 @@
         <f aca="false">RIGHT(B58,3)</f>
         <v>svg</v>
       </c>
+      <c r="F58" s="1" t="n">
+        <v>63.546</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
@@ -3248,6 +3403,9 @@
         <f aca="false">RIGHT(B59,3)</f>
         <v>svg</v>
       </c>
+      <c r="F59" s="0" t="n">
+        <v>187.56</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
@@ -3266,6 +3424,9 @@
         <f aca="false">RIGHT(B60,3)</f>
         <v>svg</v>
       </c>
+      <c r="F60" s="0" t="n">
+        <v>159.609</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
@@ -3284,6 +3445,9 @@
         <f aca="false">RIGHT(B61,3)</f>
         <v>svg</v>
       </c>
+      <c r="F61" s="0" t="n">
+        <v>63.546</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
@@ -3302,6 +3466,9 @@
         <f aca="false">RIGHT(B62,3)</f>
         <v>svg</v>
       </c>
+      <c r="F62" s="0" t="n">
+        <v>63.546</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
@@ -3320,6 +3487,9 @@
         <f aca="false">RIGHT(B63,3)</f>
         <v>svg</v>
       </c>
+      <c r="F63" s="0" t="n">
+        <v>26.02</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
@@ -3338,6 +3508,9 @@
         <f aca="false">RIGHT(B64,3)</f>
         <v>svg</v>
       </c>
+      <c r="F64" s="0" t="n">
+        <v>26.02</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
@@ -3374,6 +3547,9 @@
         <f aca="false">RIGHT(B66,3)</f>
         <v>svg</v>
       </c>
+      <c r="F66" s="0" t="n">
+        <v>2.014</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
@@ -3392,6 +3568,9 @@
         <f aca="false">RIGHT(B67,3)</f>
         <v>svg</v>
       </c>
+      <c r="F67" s="0" t="n">
+        <v>92.011</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
@@ -3428,6 +3607,9 @@
         <f aca="false">RIGHT(B69,3)</f>
         <v>svg</v>
       </c>
+      <c r="F69" s="0" t="n">
+        <v>46.07</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
@@ -3446,91 +3628,106 @@
         <f aca="false">RIGHT(B70,3)</f>
         <v>svg</v>
       </c>
+      <c r="F70" s="0" t="n">
+        <v>28.05</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B71" s="0" t="s">
         <v>213</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="E71" s="0" t="str">
         <f aca="false">RIGHT(B71,3)</f>
-        <v>txt</v>
+        <v>svg</v>
+      </c>
+      <c r="F71" s="0" t="n">
+        <v>18.998</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="E72" s="0" t="str">
         <f aca="false">RIGHT(B72,3)</f>
         <v>svg</v>
       </c>
+      <c r="F72" s="0" t="n">
+        <v>18.998</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="E73" s="0" t="str">
         <f aca="false">RIGHT(B73,3)</f>
         <v>svg</v>
       </c>
+      <c r="F73" s="0" t="n">
+        <v>18.998</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="E74" s="0" t="str">
         <f aca="false">RIGHT(B74,3)</f>
         <v>svg</v>
       </c>
+      <c r="F74" s="0" t="n">
+        <v>18.998</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="E75" s="0" t="str">
         <f aca="false">RIGHT(B75,3)</f>
@@ -3539,88 +3736,100 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="n">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="E76" s="0" t="str">
         <f aca="false">RIGHT(B76,3)</f>
         <v>svg</v>
       </c>
+      <c r="F76" s="1" t="n">
+        <v>92.0938</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="E77" s="0" t="str">
         <f aca="false">RIGHT(B77,3)</f>
         <v>svg</v>
       </c>
+      <c r="F77" s="0" t="n">
+        <v>196.967</v>
+      </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="n">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="E78" s="0" t="str">
         <f aca="false">RIGHT(B78,3)</f>
         <v>svg</v>
       </c>
+      <c r="F78" s="0" t="n">
+        <v>196.967</v>
+      </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="E79" s="0" t="str">
         <f aca="false">RIGHT(B79,3)</f>
         <v>svg</v>
       </c>
+      <c r="F79" s="0" t="n">
+        <v>196.967</v>
+      </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="E80" s="0" t="str">
         <f aca="false">RIGHT(B80,3)</f>
@@ -3629,340 +3838,394 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="E81" s="0" t="str">
         <f aca="false">RIGHT(B81,3)</f>
         <v>svg</v>
       </c>
+      <c r="F81" s="1" t="n">
+        <v>4.0026</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="E82" s="0" t="str">
         <f aca="false">RIGHT(B82,3)</f>
         <v>svg</v>
       </c>
+      <c r="F82" s="1" t="n">
+        <v>4.0026</v>
+      </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="n">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="E83" s="0" t="str">
         <f aca="false">RIGHT(B83,3)</f>
         <v>svg</v>
       </c>
+      <c r="F83" s="1" t="n">
+        <v>36.46</v>
+      </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="E84" s="0" t="str">
         <f aca="false">RIGHT(B84,3)</f>
         <v>svg</v>
       </c>
+      <c r="F84" s="1" t="n">
+        <v>36.46</v>
+      </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E85" s="0" t="str">
         <f aca="false">RIGHT(B85,3)</f>
         <v>svg</v>
       </c>
+      <c r="F85" s="1" t="n">
+        <v>1.0079</v>
+      </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="n">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E86" s="0" t="str">
         <f aca="false">RIGHT(B86,3)</f>
         <v>svg</v>
       </c>
+      <c r="F86" s="1" t="n">
+        <v>80.91</v>
+      </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="n">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="E87" s="0" t="str">
         <f aca="false">RIGHT(B87,3)</f>
         <v>svg</v>
       </c>
+      <c r="F87" s="1" t="n">
+        <v>80.91</v>
+      </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="n">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="E88" s="0" t="str">
         <f aca="false">RIGHT(B88,3)</f>
         <v>svg</v>
       </c>
+      <c r="F88" s="1" t="n">
+        <v>27.0253</v>
+      </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="E89" s="0" t="str">
         <f aca="false">RIGHT(B89,3)</f>
         <v>svg</v>
       </c>
+      <c r="F89" s="1" t="n">
+        <v>27.0253</v>
+      </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="n">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="E90" s="0" t="str">
         <f aca="false">RIGHT(B90,3)</f>
         <v>svg</v>
       </c>
+      <c r="F90" s="1" t="n">
+        <v>20.01</v>
+      </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="n">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="E91" s="0" t="str">
         <f aca="false">RIGHT(B91,3)</f>
         <v>svg</v>
       </c>
+      <c r="F91" s="1" t="n">
+        <v>127.911</v>
+      </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="n">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="E92" s="0" t="str">
         <f aca="false">RIGHT(B92,3)</f>
         <v>svg</v>
       </c>
+      <c r="F92" s="1" t="n">
+        <v>1.0079</v>
+      </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="E93" s="0" t="str">
         <f aca="false">RIGHT(B93,3)</f>
         <v>svg</v>
       </c>
+      <c r="F93" s="1" t="n">
+        <v>34.0147</v>
+      </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="n">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="D94" s="0" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="E94" s="0" t="str">
         <f aca="false">RIGHT(B94,3)</f>
         <v>svg</v>
       </c>
+      <c r="F94" s="1" t="n">
+        <v>34.1</v>
+      </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="D95" s="0" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="E95" s="0" t="str">
         <f aca="false">RIGHT(B95,3)</f>
         <v>svg</v>
       </c>
+      <c r="F95" s="1" t="n">
+        <v>1.0079</v>
+      </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="n">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="D96" s="0" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="E96" s="0" t="str">
         <f aca="false">RIGHT(B96,3)</f>
         <v>svg</v>
       </c>
+      <c r="F96" s="1" t="n">
+        <v>19.0232</v>
+      </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="n">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="E97" s="0" t="str">
         <f aca="false">RIGHT(B97,3)</f>
         <v>svg</v>
       </c>
+      <c r="F97" s="0" t="n">
+        <v>17.008</v>
+      </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="n">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="D98" s="0" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="E98" s="0" t="str">
         <f aca="false">RIGHT(B98,3)</f>
         <v>svg</v>
       </c>
+      <c r="F98" s="1" t="n">
+        <v>17.008</v>
+      </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="n">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D99" s="0" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="E99" s="0" t="str">
         <f aca="false">RIGHT(B99,3)</f>
@@ -3971,16 +4234,16 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="n">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="E100" s="0" t="str">
         <f aca="false">RIGHT(B100,3)</f>
@@ -3989,394 +4252,457 @@
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="n">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="D101" s="0" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="E101" s="0" t="str">
         <f aca="false">RIGHT(B101,3)</f>
         <v>svg</v>
       </c>
+      <c r="F101" s="1" t="n">
+        <v>126.904</v>
+      </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="n">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="E102" s="0" t="str">
         <f aca="false">RIGHT(B102,3)</f>
         <v>svg</v>
       </c>
+      <c r="F102" s="0" t="n">
+        <v>126.904</v>
+      </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="n">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="D103" s="0" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="E103" s="0" t="str">
         <f aca="false">RIGHT(B103,3)</f>
         <v>svg</v>
       </c>
+      <c r="F103" s="0" t="n">
+        <v>126.904</v>
+      </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="n">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="D104" s="0" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="E104" s="0" t="str">
         <f aca="false">RIGHT(B104,3)</f>
         <v>svg</v>
       </c>
+      <c r="F104" s="0" t="n">
+        <v>55.845</v>
+      </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="n">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="D105" s="0" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="E105" s="0" t="str">
         <f aca="false">RIGHT(B105,3)</f>
         <v>svg</v>
       </c>
+      <c r="F105" s="0" t="n">
+        <v>151.908</v>
+      </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="n">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="D106" s="0" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="E106" s="0" t="str">
         <f aca="false">RIGHT(B106,3)</f>
         <v>svg</v>
       </c>
+      <c r="F106" s="0" t="n">
+        <v>55.845</v>
+      </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="n">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="D107" s="0" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="E107" s="0" t="str">
         <f aca="false">RIGHT(B107,3)</f>
         <v>svg</v>
       </c>
+      <c r="F107" s="0" t="n">
+        <v>55.845</v>
+      </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="n">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="D108" s="0" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="E108" s="0" t="str">
         <f aca="false">RIGHT(B108,3)</f>
         <v>svg</v>
       </c>
+      <c r="F108" s="0" t="n">
+        <v>55.845</v>
+      </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="n">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="D109" s="0" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="E109" s="0" t="str">
         <f aca="false">RIGHT(B109,3)</f>
         <v>svg</v>
       </c>
+      <c r="F109" s="0" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="n">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="D110" s="0" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="E110" s="0" t="str">
         <f aca="false">RIGHT(B110,3)</f>
         <v>svg</v>
       </c>
+      <c r="F110" s="0" t="n">
+        <v>89</v>
+      </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="n">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="E111" s="0" t="str">
         <f aca="false">RIGHT(B111,3)</f>
         <v>svg</v>
       </c>
+      <c r="F111" s="0" t="n">
+        <v>461.01</v>
+      </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="n">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D112" s="0" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="E112" s="0" t="str">
         <f aca="false">RIGHT(B112,3)</f>
         <v>svg</v>
       </c>
+      <c r="F112" s="0" t="n">
+        <v>207.2</v>
+      </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="n">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="D113" s="0" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="E113" s="0" t="str">
         <f aca="false">RIGHT(B113,3)</f>
         <v>svg</v>
       </c>
+      <c r="F113" s="0" t="n">
+        <v>207.2</v>
+      </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="n">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="D114" s="0" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="E114" s="0" t="str">
         <f aca="false">RIGHT(B114,3)</f>
         <v>svg</v>
       </c>
+      <c r="F114" s="0" t="n">
+        <v>42.394</v>
+      </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="n">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="E115" s="0" t="str">
         <f aca="false">RIGHT(B115,3)</f>
         <v>svg</v>
       </c>
+      <c r="F115" s="0" t="n">
+        <v>23.95</v>
+      </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="n">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="E116" s="0" t="str">
         <f aca="false">RIGHT(B116,3)</f>
         <v>svg</v>
       </c>
+      <c r="F116" s="0" t="n">
+        <v>6.941</v>
+      </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="n">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="D117" s="0" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="E117" s="0" t="str">
         <f aca="false">RIGHT(B117,3)</f>
         <v>svg</v>
       </c>
+      <c r="F117" s="0" t="n">
+        <v>6.941</v>
+      </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="n">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B118" s="0" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="D118" s="0" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="E118" s="0" t="str">
         <f aca="false">RIGHT(B118,3)</f>
         <v>svg</v>
       </c>
+      <c r="F118" s="0" t="n">
+        <v>68.946</v>
+      </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="n">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="D119" s="0" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="E119" s="0" t="str">
         <f aca="false">RIGHT(B119,3)</f>
         <v>svg</v>
       </c>
+      <c r="F119" s="0" t="n">
+        <v>45.95</v>
+      </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="n">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B120" s="0" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="D120" s="0" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="E120" s="0" t="str">
         <f aca="false">RIGHT(B120,3)</f>
         <v>svg</v>
       </c>
+      <c r="F120" s="0" t="n">
+        <v>6.941</v>
+      </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="n">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="D121" s="0" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="E121" s="0" t="str">
         <f aca="false">RIGHT(B121,3)</f>
         <v>svg</v>
       </c>
+      <c r="F121" s="0" t="n">
+        <v>24.305</v>
+      </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="n">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B122" s="0" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="D122" s="0" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="E122" s="0" t="str">
         <f aca="false">RIGHT(B122,3)</f>
@@ -4385,16 +4711,16 @@
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="n">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B123" s="0" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="D123" s="0" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="E123" s="0" t="str">
         <f aca="false">RIGHT(B123,3)</f>
@@ -4403,16 +4729,16 @@
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="n">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B124" s="0" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C124" s="0" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="D124" s="0" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="E124" s="0" t="str">
         <f aca="false">RIGHT(B124,3)</f>
@@ -4421,16 +4747,16 @@
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="n">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B125" s="0" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="C125" s="0" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="D125" s="0" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="E125" s="0" t="str">
         <f aca="false">RIGHT(B125,3)</f>
@@ -4439,16 +4765,16 @@
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="n">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B126" s="0" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="D126" s="0" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="E126" s="0" t="str">
         <f aca="false">RIGHT(B126,3)</f>
@@ -4457,16 +4783,16 @@
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="n">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B127" s="0" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="D127" s="0" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="E127" s="0" t="str">
         <f aca="false">RIGHT(B127,3)</f>
@@ -4475,16 +4801,16 @@
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="n">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B128" s="0" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="D128" s="0" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="E128" s="0" t="str">
         <f aca="false">RIGHT(B128,3)</f>
@@ -4493,16 +4819,16 @@
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="n">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B129" s="0" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="D129" s="0" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="E129" s="0" t="str">
         <f aca="false">RIGHT(B129,3)</f>
@@ -4511,16 +4837,16 @@
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="n">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B130" s="0" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="D130" s="0" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="E130" s="0" t="str">
         <f aca="false">RIGHT(B130,3)</f>
@@ -4529,16 +4855,16 @@
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="n">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B131" s="0" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="D131" s="0" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="E131" s="0" t="str">
         <f aca="false">RIGHT(B131,3)</f>
@@ -4547,16 +4873,16 @@
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="n">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B132" s="0" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="C132" s="0" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="D132" s="0" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="E132" s="0" t="str">
         <f aca="false">RIGHT(B132,3)</f>
@@ -4565,16 +4891,16 @@
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="n">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B133" s="0" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="C133" s="0" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="D133" s="0" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="E133" s="0" t="str">
         <f aca="false">RIGHT(B133,3)</f>
@@ -4583,16 +4909,16 @@
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="n">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B134" s="0" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="D134" s="0" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="E134" s="0" t="str">
         <f aca="false">RIGHT(B134,3)</f>
@@ -4601,16 +4927,16 @@
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="n">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B135" s="0" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="C135" s="0" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D135" s="0" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="E135" s="0" t="str">
         <f aca="false">RIGHT(B135,3)</f>
@@ -4619,16 +4945,16 @@
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="n">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B136" s="0" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="D136" s="0" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="E136" s="0" t="str">
         <f aca="false">RIGHT(B136,3)</f>
@@ -4637,16 +4963,16 @@
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="n">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B137" s="0" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="C137" s="0" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="D137" s="0" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="E137" s="0" t="str">
         <f aca="false">RIGHT(B137,3)</f>
@@ -4655,16 +4981,16 @@
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="n">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B138" s="0" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="D138" s="0" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="E138" s="0" t="str">
         <f aca="false">RIGHT(B138,3)</f>
@@ -4673,16 +4999,16 @@
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="n">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B139" s="0" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="D139" s="0" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="E139" s="0" t="str">
         <f aca="false">RIGHT(B139,3)</f>
@@ -4691,16 +5017,16 @@
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="n">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B140" s="0" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="C140" s="0" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="D140" s="0" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="E140" s="0" t="str">
         <f aca="false">RIGHT(B140,3)</f>
@@ -4709,16 +5035,16 @@
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="n">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B141" s="0" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="C141" s="0" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="D141" s="0" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="E141" s="0" t="str">
         <f aca="false">RIGHT(B141,3)</f>
@@ -4727,16 +5053,16 @@
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="n">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B142" s="0" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="C142" s="0" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="D142" s="0" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="E142" s="0" t="str">
         <f aca="false">RIGHT(B142,3)</f>
@@ -4745,16 +5071,16 @@
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="n">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B143" s="0" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="C143" s="0" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="D143" s="0" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="E143" s="0" t="str">
         <f aca="false">RIGHT(B143,3)</f>
@@ -4763,16 +5089,16 @@
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="n">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B144" s="0" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="C144" s="0" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="D144" s="0" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="E144" s="0" t="str">
         <f aca="false">RIGHT(B144,3)</f>
@@ -4781,16 +5107,16 @@
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="n">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B145" s="0" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="C145" s="0" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="D145" s="0" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="E145" s="0" t="str">
         <f aca="false">RIGHT(B145,3)</f>
@@ -4799,16 +5125,16 @@
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="n">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B146" s="0" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="C146" s="0" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="D146" s="0" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="E146" s="0" t="str">
         <f aca="false">RIGHT(B146,3)</f>
@@ -4817,16 +5143,16 @@
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="n">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B147" s="0" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="C147" s="0" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="D147" s="0" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="E147" s="0" t="str">
         <f aca="false">RIGHT(B147,3)</f>
@@ -4835,16 +5161,16 @@
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="n">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B148" s="0" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="C148" s="0" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="D148" s="0" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="E148" s="0" t="str">
         <f aca="false">RIGHT(B148,3)</f>
@@ -4853,16 +5179,16 @@
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="n">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B149" s="0" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="C149" s="0" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="D149" s="0" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="E149" s="0" t="str">
         <f aca="false">RIGHT(B149,3)</f>
@@ -4871,16 +5197,16 @@
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="n">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B150" s="0" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="C150" s="0" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="D150" s="0" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="E150" s="0" t="str">
         <f aca="false">RIGHT(B150,3)</f>
@@ -4889,16 +5215,16 @@
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="n">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B151" s="0" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="C151" s="0" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="D151" s="0" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="E151" s="0" t="str">
         <f aca="false">RIGHT(B151,3)</f>
@@ -4907,16 +5233,16 @@
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="n">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B152" s="0" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="C152" s="0" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="D152" s="0" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="E152" s="0" t="str">
         <f aca="false">RIGHT(B152,3)</f>
@@ -4925,16 +5251,16 @@
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="n">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B153" s="0" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="C153" s="0" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="D153" s="0" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="E153" s="0" t="str">
         <f aca="false">RIGHT(B153,3)</f>
@@ -4943,16 +5269,16 @@
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="n">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B154" s="0" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="C154" s="0" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="D154" s="0" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="E154" s="0" t="str">
         <f aca="false">RIGHT(B154,3)</f>
@@ -4961,16 +5287,16 @@
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="n">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B155" s="0" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="C155" s="0" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="D155" s="0" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="E155" s="0" t="str">
         <f aca="false">RIGHT(B155,3)</f>
@@ -4979,16 +5305,16 @@
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="n">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B156" s="0" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="C156" s="0" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="D156" s="0" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="E156" s="0" t="str">
         <f aca="false">RIGHT(B156,3)</f>
@@ -4997,16 +5323,16 @@
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="n">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B157" s="0" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="C157" s="0" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="D157" s="0" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="E157" s="0" t="str">
         <f aca="false">RIGHT(B157,3)</f>
@@ -5015,16 +5341,16 @@
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="n">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B158" s="0" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="C158" s="0" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="D158" s="0" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="E158" s="0" t="str">
         <f aca="false">RIGHT(B158,3)</f>
@@ -5033,16 +5359,16 @@
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="n">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B159" s="0" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="C159" s="0" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="D159" s="0" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="E159" s="0" t="str">
         <f aca="false">RIGHT(B159,3)</f>
@@ -5051,16 +5377,16 @@
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="n">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B160" s="0" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="C160" s="0" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="D160" s="0" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="E160" s="0" t="str">
         <f aca="false">RIGHT(B160,3)</f>
@@ -5069,16 +5395,16 @@
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="n">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B161" s="0" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="C161" s="0" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="D161" s="0" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="E161" s="0" t="str">
         <f aca="false">RIGHT(B161,3)</f>
@@ -5087,16 +5413,16 @@
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="n">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B162" s="0" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="C162" s="0" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="D162" s="0" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="E162" s="0" t="str">
         <f aca="false">RIGHT(B162,3)</f>
@@ -5105,16 +5431,16 @@
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="n">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B163" s="0" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="C163" s="0" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="D163" s="0" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="E163" s="0" t="str">
         <f aca="false">RIGHT(B163,3)</f>
@@ -5123,16 +5449,16 @@
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="n">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B164" s="0" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="C164" s="0" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="D164" s="0" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="E164" s="0" t="str">
         <f aca="false">RIGHT(B164,3)</f>
@@ -5141,16 +5467,16 @@
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="n">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B165" s="0" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="C165" s="0" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="D165" s="0" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="E165" s="0" t="str">
         <f aca="false">RIGHT(B165,3)</f>
@@ -5159,16 +5485,16 @@
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="n">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B166" s="0" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="C166" s="0" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="D166" s="0" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="E166" s="0" t="str">
         <f aca="false">RIGHT(B166,3)</f>
@@ -5177,16 +5503,16 @@
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="n">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B167" s="0" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="C167" s="0" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="D167" s="0" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="E167" s="0" t="str">
         <f aca="false">RIGHT(B167,3)</f>
@@ -5195,16 +5521,16 @@
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="n">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B168" s="0" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="C168" s="0" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="D168" s="0" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="E168" s="0" t="str">
         <f aca="false">RIGHT(B168,3)</f>
@@ -5213,16 +5539,16 @@
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="n">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B169" s="0" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="C169" s="0" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="D169" s="0" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="E169" s="0" t="str">
         <f aca="false">RIGHT(B169,3)</f>
@@ -5231,16 +5557,16 @@
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="n">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B170" s="0" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="C170" s="0" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="D170" s="0" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="E170" s="0" t="str">
         <f aca="false">RIGHT(B170,3)</f>
@@ -5249,16 +5575,16 @@
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="n">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B171" s="0" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="C171" s="0" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="D171" s="0" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="E171" s="0" t="str">
         <f aca="false">RIGHT(B171,3)</f>
@@ -5267,16 +5593,16 @@
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="n">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B172" s="0" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="C172" s="0" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="D172" s="0" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="E172" s="0" t="str">
         <f aca="false">RIGHT(B172,3)</f>
@@ -5285,16 +5611,16 @@
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="n">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B173" s="0" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="C173" s="0" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="D173" s="0" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="E173" s="0" t="str">
         <f aca="false">RIGHT(B173,3)</f>
@@ -5303,16 +5629,16 @@
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="n">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B174" s="0" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="C174" s="0" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="D174" s="0" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="E174" s="0" t="str">
         <f aca="false">RIGHT(B174,3)</f>
@@ -5321,16 +5647,16 @@
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="n">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B175" s="0" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="C175" s="0" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="D175" s="0" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="E175" s="0" t="str">
         <f aca="false">RIGHT(B175,3)</f>
@@ -5339,16 +5665,16 @@
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="n">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B176" s="0" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="C176" s="0" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="D176" s="0" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="E176" s="0" t="str">
         <f aca="false">RIGHT(B176,3)</f>
@@ -5357,16 +5683,16 @@
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="n">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B177" s="0" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="C177" s="0" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="D177" s="0" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="E177" s="0" t="str">
         <f aca="false">RIGHT(B177,3)</f>
@@ -5375,16 +5701,16 @@
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="n">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B178" s="0" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="C178" s="0" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="D178" s="0" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="E178" s="0" t="str">
         <f aca="false">RIGHT(B178,3)</f>
@@ -5393,16 +5719,16 @@
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="n">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B179" s="0" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="C179" s="0" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="D179" s="0" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="E179" s="0" t="str">
         <f aca="false">RIGHT(B179,3)</f>
@@ -5411,16 +5737,16 @@
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="n">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B180" s="0" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="C180" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="D180" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="E180" s="0" t="str">
         <f aca="false">RIGHT(B180,3)</f>
@@ -5429,16 +5755,16 @@
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="n">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B181" s="0" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="C181" s="0" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="D181" s="0" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="E181" s="0" t="str">
         <f aca="false">RIGHT(B181,3)</f>
@@ -5447,16 +5773,16 @@
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="n">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B182" s="0" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="C182" s="0" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="D182" s="0" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="E182" s="0" t="str">
         <f aca="false">RIGHT(B182,3)</f>
@@ -5465,16 +5791,16 @@
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="n">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B183" s="0" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="C183" s="0" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="D183" s="0" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="E183" s="0" t="str">
         <f aca="false">RIGHT(B183,3)</f>
@@ -5483,16 +5809,16 @@
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="n">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B184" s="0" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="C184" s="0" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="D184" s="0" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="E184" s="0" t="str">
         <f aca="false">RIGHT(B184,3)</f>
@@ -5501,16 +5827,16 @@
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="n">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B185" s="0" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="C185" s="0" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="D185" s="0" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="E185" s="0" t="str">
         <f aca="false">RIGHT(B185,3)</f>
@@ -5519,16 +5845,16 @@
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="n">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B186" s="0" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="C186" s="0" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="D186" s="0" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="E186" s="0" t="str">
         <f aca="false">RIGHT(B186,3)</f>
@@ -5537,16 +5863,16 @@
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="n">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B187" s="0" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="C187" s="0" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="D187" s="0" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="E187" s="0" t="str">
         <f aca="false">RIGHT(B187,3)</f>
@@ -5555,16 +5881,16 @@
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="n">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B188" s="0" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="C188" s="0" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="D188" s="0" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="E188" s="0" t="str">
         <f aca="false">RIGHT(B188,3)</f>
@@ -5573,16 +5899,16 @@
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="n">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B189" s="0" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="C189" s="0" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="D189" s="0" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="E189" s="0" t="str">
         <f aca="false">RIGHT(B189,3)</f>
@@ -5591,16 +5917,16 @@
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="n">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B190" s="0" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="C190" s="0" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="D190" s="0" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="E190" s="0" t="str">
         <f aca="false">RIGHT(B190,3)</f>
@@ -5609,16 +5935,16 @@
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="n">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B191" s="0" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="C191" s="0" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="D191" s="0" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="E191" s="0" t="str">
         <f aca="false">RIGHT(B191,3)</f>
@@ -5627,16 +5953,16 @@
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="n">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B192" s="0" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="C192" s="0" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="D192" s="0" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="E192" s="0" t="str">
         <f aca="false">RIGHT(B192,3)</f>
@@ -5645,16 +5971,16 @@
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="n">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B193" s="0" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="C193" s="0" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="D193" s="0" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="E193" s="0" t="str">
         <f aca="false">RIGHT(B193,3)</f>
@@ -5663,16 +5989,16 @@
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="n">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B194" s="0" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="C194" s="0" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="D194" s="0" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="E194" s="0" t="str">
         <f aca="false">RIGHT(B194,3)</f>
@@ -5681,16 +6007,16 @@
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="n">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B195" s="0" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="C195" s="0" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="D195" s="0" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="E195" s="0" t="str">
         <f aca="false">RIGHT(B195,3)</f>
@@ -5699,16 +6025,16 @@
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="n">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B196" s="0" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="C196" s="0" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="D196" s="0" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="E196" s="0" t="str">
         <f aca="false">RIGHT(B196,3)</f>
@@ -5717,16 +6043,16 @@
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="n">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B197" s="0" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="C197" s="0" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="D197" s="0" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="E197" s="0" t="str">
         <f aca="false">RIGHT(B197,3)</f>
@@ -5735,16 +6061,16 @@
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="n">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B198" s="0" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="C198" s="0" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="D198" s="0" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="E198" s="0" t="str">
         <f aca="false">RIGHT(B198,3)</f>
@@ -5753,16 +6079,16 @@
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="n">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B199" s="0" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c r="C199" s="0" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="D199" s="0" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="E199" s="0" t="str">
         <f aca="false">RIGHT(B199,3)</f>
@@ -5771,16 +6097,16 @@
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="n">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B200" s="0" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="C200" s="0" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="D200" s="0" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="E200" s="0" t="str">
         <f aca="false">RIGHT(B200,3)</f>
@@ -5789,16 +6115,16 @@
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="n">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B201" s="0" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="C201" s="0" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="D201" s="0" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="E201" s="0" t="str">
         <f aca="false">RIGHT(B201,3)</f>
@@ -5807,16 +6133,16 @@
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="n">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B202" s="0" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="C202" s="0" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="D202" s="0" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="E202" s="0" t="str">
         <f aca="false">RIGHT(B202,3)</f>
@@ -5825,16 +6151,16 @@
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="n">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B203" s="0" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="C203" s="0" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="D203" s="0" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="E203" s="0" t="str">
         <f aca="false">RIGHT(B203,3)</f>
@@ -5843,16 +6169,16 @@
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="n">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B204" s="0" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="C204" s="0" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="D204" s="0" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="E204" s="0" t="str">
         <f aca="false">RIGHT(B204,3)</f>
@@ -5861,16 +6187,16 @@
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="n">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B205" s="0" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="C205" s="0" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="D205" s="0" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="E205" s="0" t="str">
         <f aca="false">RIGHT(B205,3)</f>
@@ -5879,16 +6205,16 @@
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="n">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B206" s="0" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="C206" s="0" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="D206" s="0" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="E206" s="0" t="str">
         <f aca="false">RIGHT(B206,3)</f>
@@ -5897,16 +6223,16 @@
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="n">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B207" s="0" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="C207" s="0" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="D207" s="0" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="E207" s="0" t="str">
         <f aca="false">RIGHT(B207,3)</f>
@@ -5915,16 +6241,16 @@
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="n">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B208" s="0" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="C208" s="0" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="D208" s="0" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="E208" s="0" t="str">
         <f aca="false">RIGHT(B208,3)</f>
@@ -5933,16 +6259,16 @@
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="n">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B209" s="0" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="C209" s="0" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="D209" s="0" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="E209" s="0" t="str">
         <f aca="false">RIGHT(B209,3)</f>
@@ -5951,16 +6277,16 @@
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="n">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B210" s="0" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="C210" s="0" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="D210" s="0" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="E210" s="0" t="str">
         <f aca="false">RIGHT(B210,3)</f>
@@ -5969,16 +6295,16 @@
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="n">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B211" s="0" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
       <c r="C211" s="0" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="D211" s="0" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="E211" s="0" t="str">
         <f aca="false">RIGHT(B211,3)</f>
@@ -5987,16 +6313,16 @@
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="n">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B212" s="0" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="C212" s="0" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c r="D212" s="0" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="E212" s="0" t="str">
         <f aca="false">RIGHT(B212,3)</f>
@@ -6005,16 +6331,16 @@
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="n">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B213" s="0" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="C213" s="0" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="D213" s="0" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="E213" s="0" t="str">
         <f aca="false">RIGHT(B213,3)</f>
@@ -6023,16 +6349,16 @@
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="n">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B214" s="0" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="C214" s="0" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="D214" s="0" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="E214" s="0" t="str">
         <f aca="false">RIGHT(B214,3)</f>
@@ -6041,16 +6367,16 @@
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="n">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B215" s="0" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="C215" s="0" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="D215" s="0" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="E215" s="0" t="str">
         <f aca="false">RIGHT(B215,3)</f>
@@ -6059,16 +6385,16 @@
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="n">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B216" s="0" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="C216" s="0" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="D216" s="0" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="E216" s="0" t="str">
         <f aca="false">RIGHT(B216,3)</f>
@@ -6077,16 +6403,16 @@
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="n">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B217" s="0" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="C217" s="0" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="D217" s="0" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="E217" s="0" t="str">
         <f aca="false">RIGHT(B217,3)</f>
@@ -6095,16 +6421,16 @@
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="n">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B218" s="0" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="C218" s="0" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="D218" s="0" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="E218" s="0" t="str">
         <f aca="false">RIGHT(B218,3)</f>
@@ -6113,16 +6439,16 @@
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="n">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B219" s="0" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="C219" s="0" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
       <c r="D219" s="0" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="E219" s="0" t="str">
         <f aca="false">RIGHT(B219,3)</f>
@@ -6131,16 +6457,16 @@
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="n">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B220" s="0" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="C220" s="0" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="D220" s="0" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="E220" s="0" t="str">
         <f aca="false">RIGHT(B220,3)</f>
@@ -6149,16 +6475,16 @@
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="n">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B221" s="0" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="C221" s="0" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="D221" s="0" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="E221" s="0" t="str">
         <f aca="false">RIGHT(B221,3)</f>
@@ -6167,16 +6493,16 @@
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="n">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B222" s="0" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="C222" s="0" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="D222" s="0" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="E222" s="0" t="str">
         <f aca="false">RIGHT(B222,3)</f>
@@ -6185,16 +6511,16 @@
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="n">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B223" s="0" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="C223" s="0" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="D223" s="0" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="E223" s="0" t="str">
         <f aca="false">RIGHT(B223,3)</f>
@@ -6203,16 +6529,16 @@
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="n">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B224" s="0" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="C224" s="0" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="D224" s="0" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="E224" s="0" t="str">
         <f aca="false">RIGHT(B224,3)</f>
@@ -6221,16 +6547,16 @@
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="n">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B225" s="0" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="C225" s="0" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="D225" s="0" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="E225" s="0" t="str">
         <f aca="false">RIGHT(B225,3)</f>
@@ -6239,16 +6565,16 @@
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="n">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B226" s="0" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="C226" s="0" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="D226" s="0" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="E226" s="0" t="str">
         <f aca="false">RIGHT(B226,3)</f>
@@ -6257,37 +6583,19 @@
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="n">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B227" s="0" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="C227" s="0" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="D227" s="0" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="E227" s="0" t="str">
         <f aca="false">RIGHT(B227,3)</f>
-        <v>svg</v>
-      </c>
-    </row>
-    <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A228" s="0" t="n">
-        <v>227</v>
-      </c>
-      <c r="B228" s="0" t="s">
-        <v>682</v>
-      </c>
-      <c r="C228" s="0" t="s">
-        <v>683</v>
-      </c>
-      <c r="D228" s="0" t="s">
-        <v>684</v>
-      </c>
-      <c r="E228" s="0" t="str">
-        <f aca="false">RIGHT(B228,3)</f>
         <v>svg</v>
       </c>
     </row>

</xml_diff>